<commit_message>
Function Point Update for Tickets
</commit_message>
<xml_diff>
--- a/Use Case/Functionpoint_overview.xlsx
+++ b/Use Case/Functionpoint_overview.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix Morsbach\Documents\GitHub\documents\Use Case\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\GitHub\documents\Use Case\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,15 +19,12 @@
     <sheet name="Edit personal Data" sheetId="5" r:id="rId5"/>
     <sheet name="Manage User Data" sheetId="6" r:id="rId6"/>
     <sheet name="Give Feedback" sheetId="7" r:id="rId7"/>
-    <sheet name="Give Support" sheetId="8" r:id="rId8"/>
+    <sheet name="Answer Ticket" sheetId="8" r:id="rId8"/>
     <sheet name="Check Game Results" sheetId="9" r:id="rId9"/>
     <sheet name="Bet on Win" sheetId="10" r:id="rId10"/>
     <sheet name="Wager Bet" sheetId="12" r:id="rId11"/>
     <sheet name="Buy - Get Reward" sheetId="11" r:id="rId12"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId13"/>
-  </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="51">
   <si>
     <t>Login</t>
   </si>
@@ -127,9 +124,6 @@
     <t>UC: Buy / Get Reward</t>
   </si>
   <si>
-    <t>UC: Give Support</t>
-  </si>
-  <si>
     <t>UC: Give Feedback</t>
   </si>
   <si>
@@ -188,13 +182,19 @@
   </si>
   <si>
     <t>Expectation</t>
+  </si>
+  <si>
+    <t>UC: Answer Ticket</t>
+  </si>
+  <si>
+    <t>Adjust Function manually</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,6 +233,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -260,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -289,6 +296,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -482,10 +490,10 @@
                   <c:v>84.48</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>65</c:v>
+                  <c:v>71.099999999999994</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>70</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -515,7 +523,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -530,11 +538,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="374178128"/>
-        <c:axId val="374171464"/>
+        <c:axId val="395384904"/>
+        <c:axId val="395386080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="374178128"/>
+        <c:axId val="395384904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="60"/>
@@ -648,12 +656,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374171464"/>
+        <c:crossAx val="395386080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="374171464"/>
+        <c:axId val="395386080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -767,7 +775,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374178128"/>
+        <c:crossAx val="395384904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1409,100 +1417,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="UC"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="5">
-          <cell r="E5">
-            <v>3.5</v>
-          </cell>
-          <cell r="F5">
-            <v>18</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="E6">
-            <v>4</v>
-          </cell>
-          <cell r="F6">
-            <v>15.3</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="E7">
-            <v>5.5</v>
-          </cell>
-          <cell r="F7">
-            <v>17.5</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="E8">
-            <v>6</v>
-          </cell>
-          <cell r="F8">
-            <v>14.9</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="E9">
-            <v>6.5</v>
-          </cell>
-          <cell r="F9">
-            <v>49.5</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="E10">
-            <v>7</v>
-          </cell>
-          <cell r="F10">
-            <v>39.6</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="E11">
-            <v>9.5</v>
-          </cell>
-          <cell r="F11">
-            <v>30.5</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="E14">
-            <v>5.1502517567642343</v>
-          </cell>
-          <cell r="F14">
-            <v>23.4</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="E15">
-            <v>5.1502517567642343</v>
-          </cell>
-          <cell r="F15">
-            <v>23.4</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="E16">
-            <v>21.334615171803243</v>
-          </cell>
-          <cell r="F16">
-            <v>81.900000000000006</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1769,7 +1683,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1781,37 +1695,40 @@
   <sheetData>
     <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="E5" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>46</v>
-      </c>
       <c r="F5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1854,13 +1771,13 @@
         <v>1</v>
       </c>
       <c r="F7" s="11">
-        <f>SUM(C7,D7,E7)</f>
+        <f t="shared" ref="F7:F12" si="1">SUM(C7,D7,E7)</f>
         <v>5.5</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" s="13">
         <f>'Check Leaderboard'!$H$14</f>
@@ -1876,13 +1793,13 @@
         <v>0.5</v>
       </c>
       <c r="F8" s="11">
-        <f>SUM(C8,D8,E8)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" s="13">
         <f>'Edit personal Data'!$H$14</f>
@@ -1898,13 +1815,13 @@
         <v>1.5</v>
       </c>
       <c r="F9" s="11">
-        <f>SUM(C9,D9,E9)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="13">
         <f>'Manage User Data'!$H$14</f>
@@ -1920,17 +1837,17 @@
         <v>2</v>
       </c>
       <c r="F10" s="11">
-        <f>SUM(C10,D10,E10)</f>
+        <f t="shared" si="1"/>
         <v>9.5</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11" s="13">
         <f>'Give Feedback'!$H$14</f>
-        <v>65</v>
+        <v>71.099999999999994</v>
       </c>
       <c r="C11" s="3">
         <v>1.5</v>
@@ -1942,35 +1859,35 @@
         <v>0.5</v>
       </c>
       <c r="F11" s="11">
-        <f>SUM(C11,D11,E11)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" s="13">
-        <f>'Give Support'!$H$14</f>
-        <v>70</v>
+        <f>'Answer Ticket'!$H$14</f>
+        <v>99</v>
       </c>
       <c r="C12" s="3">
         <v>1.5</v>
       </c>
       <c r="D12" s="3">
-        <v>3.5</v>
+        <v>5</v>
       </c>
       <c r="E12" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" s="11">
-        <f>SUM(C12,D12,E12)</f>
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>8.5</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" s="13">
         <f>'Check Game Results'!$H$14</f>
@@ -1978,13 +1895,13 @@
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="12">
-        <f>0.2686*B13-13.04</f>
-        <v>0.90571200000000118</v>
+        <f>0.147*B13-4.9205</f>
+        <v>2.7117399999999998</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="13">
         <f>'Bet on Win'!$H$14</f>
@@ -1992,13 +1909,13 @@
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="12">
-        <f t="shared" ref="G14:G16" si="1">0.2686*B14-13.04</f>
-        <v>7.3870299999999993</v>
+        <f t="shared" ref="G14:G16" si="2">0.147*B14-4.9205</f>
+        <v>6.2588499999999998</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="13">
         <f>'Wager Bet'!$H$14</f>
@@ -2006,13 +1923,13 @@
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="12">
-        <f t="shared" si="1"/>
-        <v>10.355059999999998</v>
+        <f t="shared" si="2"/>
+        <v>7.8831999999999995</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16" s="13">
         <f>'Buy - Get Reward'!$H$14</f>
@@ -2020,8 +1937,8 @@
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="12">
-        <f t="shared" si="1"/>
-        <v>4.0698200000000035</v>
+        <f t="shared" si="2"/>
+        <v>4.4433999999999996</v>
       </c>
     </row>
     <row r="21" spans="3:11" x14ac:dyDescent="0.25">
@@ -2337,7 +2254,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2914,7 +2831,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G14" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H14">
         <v>66.88</v>
@@ -3118,7 +3035,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G14" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H14">
         <v>69.52</v>
@@ -3533,8 +3450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K62" sqref="K62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3744,7 +3661,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -3786,11 +3703,21 @@
         <v>3</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -3800,11 +3727,21 @@
         <v>4</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
@@ -3835,11 +3772,21 @@
         <v>11</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="D9" s="3">
+        <v>2</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -3849,11 +3796,21 @@
         <v>12</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -3863,15 +3820,25 @@
         <v>13</v>
       </c>
       <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="D11" s="3">
+        <v>2</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H14">
-        <v>65</v>
+        <v>71.099999999999994</v>
       </c>
     </row>
   </sheetData>
@@ -3894,7 +3861,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -3936,11 +3903,21 @@
         <v>3</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>2</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="3">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -3950,11 +3927,21 @@
         <v>4</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
@@ -3985,11 +3972,21 @@
         <v>11</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="D9" s="3">
+        <v>4</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -3999,11 +3996,21 @@
         <v>12</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -4013,15 +4020,25 @@
         <v>13</v>
       </c>
       <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="D11" s="3">
+        <v>2</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H14">
-        <v>70</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Time Log in Function Shart
</commit_message>
<xml_diff>
--- a/Use Case/Functionpoint_overview.xlsx
+++ b/Use Case/Functionpoint_overview.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="54">
   <si>
     <t>Login</t>
   </si>
@@ -188,6 +188,15 @@
   </si>
   <si>
     <t>Adjust Function manually</t>
+  </si>
+  <si>
+    <t>Begrüdung</t>
+  </si>
+  <si>
+    <t>Ausreißer</t>
+  </si>
+  <si>
+    <t>Code von Place Bet wieder verwendbar, daher Coding Aufwand deutlich geringer.</t>
   </si>
 </sst>
 </file>
@@ -241,7 +250,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,6 +260,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -267,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -288,7 +309,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -297,6 +317,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -399,7 +421,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>results</c:v>
+            <c:v>resultssemester2</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -434,6 +456,8 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
+            <c:forward val="15"/>
+            <c:backward val="50"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -523,7 +547,222 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.5</c:v>
+                  <c:v>9.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>resultsSemetser2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.2733060482037357E-2"/>
+                  <c:y val="-4.5976882200069936E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:noAutofit/>
+                  </a:bodyPr>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="75000"/>
+                            <a:lumOff val="25000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>Wager Bet - Ausreißer</a:t>
+                    </a:r>
+                  </a:p>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr/>
+                    </a:pPr>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:noAutofit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.15812642110050024"/>
+                      <c:h val="4.9162561576354673E-2"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Overview!$B$13:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>51.92</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>76.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>87.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>63.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Overview!$F$13:$F$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -538,14 +777,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="395384904"/>
-        <c:axId val="395386080"/>
+        <c:axId val="422691672"/>
+        <c:axId val="422696768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="395384904"/>
+        <c:axId val="422691672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="60"/>
+          <c:min val="50"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -656,12 +895,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="395386080"/>
+        <c:crossAx val="422696768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="395386080"/>
+        <c:axId val="422696768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -775,7 +1014,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="395384904"/>
+        <c:crossAx val="422691672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1385,15 +1624,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>38099</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>161924</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>76201</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1683,7 +1922,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1708,7 +1947,7 @@
       <c r="C4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="13" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1732,10 +1971,10 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="13">
+      <c r="A6" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="12">
         <f>Login!$H$14</f>
         <v>66.88</v>
       </c>
@@ -1748,16 +1987,16 @@
       <c r="E6" s="3">
         <v>0.5</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="10">
         <f t="shared" ref="F6" si="0">SUM(C6,D6,E6)</f>
         <v>3.5</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="12">
         <f>Register!$H$14</f>
         <v>69.52</v>
       </c>
@@ -1770,16 +2009,16 @@
       <c r="E7" s="3">
         <v>1</v>
       </c>
-      <c r="F7" s="11">
-        <f t="shared" ref="F7:F12" si="1">SUM(C7,D7,E7)</f>
+      <c r="F7" s="10">
+        <f t="shared" ref="F7:F16" si="1">SUM(C7,D7,E7)</f>
         <v>5.5</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="12">
         <f>'Check Leaderboard'!$H$14</f>
         <v>64.239999999999995</v>
       </c>
@@ -1792,16 +2031,16 @@
       <c r="E8" s="3">
         <v>0.5</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="10">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="12">
         <f>'Edit personal Data'!$H$14</f>
         <v>69.52</v>
       </c>
@@ -1814,16 +2053,16 @@
       <c r="E9" s="3">
         <v>1.5</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="10">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="12">
         <f>'Manage User Data'!$H$14</f>
         <v>84.48</v>
       </c>
@@ -1836,16 +2075,16 @@
       <c r="E10" s="3">
         <v>2</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="10">
         <f t="shared" si="1"/>
         <v>9.5</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="12">
         <f>'Give Feedback'!$H$14</f>
         <v>71.099999999999994</v>
       </c>
@@ -1858,16 +2097,16 @@
       <c r="E11" s="3">
         <v>0.5</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="10">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B12" s="12">
         <f>'Answer Ticket'!$H$14</f>
         <v>99</v>
       </c>
@@ -1875,73 +2114,121 @@
         <v>1.5</v>
       </c>
       <c r="D12" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E12" s="3">
         <v>2</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="10">
         <f t="shared" si="1"/>
-        <v>8.5</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B13" s="12">
         <f>'Check Game Results'!$H$14</f>
         <v>51.92</v>
       </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="12">
-        <f>0.147*B13-4.9205</f>
-        <v>2.7117399999999998</v>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F13" s="10">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="G13" s="11">
+        <f>0.1736*B13-6.7302</f>
+        <v>2.2831120000000009</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="12">
         <f>'Bet on Win'!$H$14</f>
         <v>76.05</v>
       </c>
-      <c r="F14" s="10"/>
-      <c r="G14" s="12">
-        <f t="shared" ref="G14:G16" si="2">0.147*B14-4.9205</f>
-        <v>6.2588499999999998</v>
+      <c r="C14" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="D14" s="3">
+        <v>5</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="10">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+      <c r="G14" s="11">
+        <f t="shared" ref="G14:G16" si="2">0.1736*B14-6.7302</f>
+        <v>6.4720800000000001</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="13">
+      <c r="B15" s="12">
         <f>'Wager Bet'!$H$14</f>
         <v>87.1</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="12">
+      <c r="C15" s="3">
+        <v>1</v>
+      </c>
+      <c r="D15" s="3">
+        <v>2</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F15" s="10">
+        <f t="shared" si="1"/>
+        <v>3.5</v>
+      </c>
+      <c r="G15" s="11">
         <f t="shared" si="2"/>
-        <v>7.8831999999999995</v>
+        <v>8.3903599999999994</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B16" s="12">
         <f>'Buy - Get Reward'!$H$14</f>
         <v>63.7</v>
       </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="12">
+      <c r="C16" s="3">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F16" s="10">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="G16" s="11">
         <f t="shared" si="2"/>
-        <v>4.4433999999999996</v>
-      </c>
-    </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
+        <v>4.3281200000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -1949,7 +2236,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -1957,7 +2244,13 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -1965,7 +2258,13 @@
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" t="s">
+        <v>53</v>
+      </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -1975,7 +2274,7 @@
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
     </row>
-    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -1985,7 +2284,7 @@
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
     </row>
-    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
@@ -1995,7 +2294,7 @@
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
     </row>
-    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C27" s="4"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -2006,27 +2305,27 @@
       <c r="J27" s="3"/>
       <c r="K27" s="9"/>
     </row>
-    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C28" s="4"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C29" s="4"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="G31" s="3"/>
     </row>
-    <row r="32" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="G32" s="3"/>
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.25">

</xml_diff>